<commit_message>
update BOM and model
</commit_message>
<xml_diff>
--- a/BOM/DataAcq-EnvironmentBoard.xlsx
+++ b/BOM/DataAcq-EnvironmentBoard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi\Git\LHR\DataAcq-EnvironmentBoard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C51500-A9FE-4BB2-9A42-7AE9B180EF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973079EE-AD21-4945-85B6-53A27C91F092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{81A77C0A-716C-4A17-92A9-26BF0F90DC4A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -38,27 +38,6 @@
     <t>P/N</t>
   </si>
   <si>
-    <t>C1,C2,C3,C5,C7</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>C0805C104M5RACTU</t>
-  </si>
-  <si>
-    <t>C4,C6</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>C0805C105K5PACTU</t>
-  </si>
-  <si>
     <t>D1,D2</t>
   </si>
   <si>
@@ -74,18 +53,9 @@
     <t>UTSVT_Connectors:Molex_MicroFit3.0_1x4xP3.00mm_PolarizingPeg_Vertical</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>Resistor_SMD:R_0805_2012Metric</t>
   </si>
   <si>
-    <t>CRCW08051K00FKEAC</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -104,39 +74,6 @@
     <t>SDR10EZPF2200</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SHT45</t>
-  </si>
-  <si>
-    <t>Sensor_Humidity:Sensirion_DFN-4_1.5x1.5mm_P0.8mm_SHT4x_NoCentralPad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHT45-AD1B-R3 </t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>FS3000-1005</t>
-  </si>
-  <si>
-    <t>FS30001005</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>LMT87DCK</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_SMD:SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>LMT87QDCKRQ1</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -171,9 +108,6 @@
   </si>
   <si>
     <t>0ZCM0010FF2G</t>
-  </si>
-  <si>
-    <t>SamacSys_Parts:FS30001005</t>
   </si>
   <si>
     <t>J1,J2,J3,J4</t>
@@ -1049,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2617CE33-6BC1-4FEF-A157-3E9A29852109}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1091,7 +1025,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -1099,104 +1033,104 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>45</v>
+      <c r="E5" s="1">
+        <v>436500244</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>436500315</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>436500244</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
-        <v>436500315</v>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -1214,108 +1148,6 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1325,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C09B32C-854C-4A59-8AA9-5D54371B8E4D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1358,104 +1190,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>